<commit_message>
estudio de 10 a 100%
</commit_message>
<xml_diff>
--- a/Docs importantes/Experimento 1/criterio1VScriterio3.xlsx
+++ b/Docs importantes/Experimento 1/criterio1VScriterio3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Desktop\Universidad\Cuarto de carrera\Segundo cuatrimestre\Prácticas\Docs importantes\Experimento 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Desktop\Universidad\Cuarto de carrera\Segundo cuatrimestre\Prácticas investigación\Docs importantes\Experimento 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EFE29A-E7DD-4C4D-A488-A3F748D7348A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70570167-88B2-4E87-9708-390FC290B50C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D6DAAA7A-F829-4C97-A67F-BF00D45AC1A6}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t>SOM-b_2_n100_m20.txt</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>CV REF</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>IGD</t>
+  </si>
+  <si>
+    <t>Time(s)</t>
   </si>
 </sst>
 </file>
@@ -217,15 +217,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -233,23 +245,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,7 +598,7 @@
   <dimension ref="A2:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,96 +621,97 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
         <f>AVERAGE(B7:B30)</f>
         <v>0.85717499431598154</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <f t="shared" ref="C3:H3" si="0">AVERAGE(C7:C30)</f>
         <v>2.6302947230595938E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <f t="shared" si="0"/>
         <v>1.3445532721463394</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <f t="shared" si="0"/>
         <v>8530.6188581680381</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <f t="shared" si="0"/>
         <v>18.833333333333332</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
         <f t="shared" si="0"/>
         <v>0.97885344723100565</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <f t="shared" si="0"/>
         <v>650.08549043728738</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>158.87799999999999</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <f>AVERAGE(I7:I30)</f>
         <v>2.8104135919600769E-2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <f t="shared" ref="C4:H4" si="1">AVERAGE(J7:J30)</f>
         <v>0.25950100626463851</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <f t="shared" si="1"/>
         <v>6.409964241117054E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <f t="shared" si="1"/>
         <v>13521.57842543016</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <f t="shared" si="1"/>
         <v>13.625</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="5">
         <f t="shared" si="1"/>
         <v>0.97912149871423715</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="5">
         <f t="shared" si="1"/>
         <v>477.18548303161015</v>
       </c>

</xml_diff>

<commit_message>
comparativa ls todas vs pareto
</commit_message>
<xml_diff>
--- a/Docs importantes/Experimento 1/criterio1VScriterio3.xlsx
+++ b/Docs importantes/Experimento 1/criterio1VScriterio3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Desktop\Universidad\Cuarto de carrera\Segundo cuatrimestre\Prácticas investigación\Docs importantes\Experimento 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Investigacion-maxima-diversidad\Docs importantes\Experimento 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70570167-88B2-4E87-9708-390FC290B50C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F95C25-4C4E-4F2B-BF4B-FF9100BB13D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D6DAAA7A-F829-4C97-A67F-BF00D45AC1A6}"/>
+    <workbookView xWindow="28680" yWindow="-2850" windowWidth="24240" windowHeight="13140" xr2:uid="{D6DAAA7A-F829-4C97-A67F-BF00D45AC1A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -601,26 +601,26 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="9" t="s">
         <v>41</v>
@@ -647,7 +647,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -683,7 +683,7 @@
         <v>158.87799999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -719,7 +719,7 @@
         <v>161.56299999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -766,7 +766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -813,7 +813,7 @@
         <v>143.54439485194999</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -860,7 +860,7 @@
         <v>94.110837399318797</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -907,7 +907,7 @@
         <v>303.39960914610202</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -954,7 +954,7 @@
         <v>171.14737307314601</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>203.43324764738799</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>195.34056899203199</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>532.76028624810795</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>107.35075415658299</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>106.34959275298699</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>190.67684258931899</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>196.40238526003401</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>540.78838443205802</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>183.14411284545</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>643.52627276272403</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>1044.7149406674801</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>160.220957309754</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>95.192697862829107</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>74.123954385461701</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>77.328445526304506</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>64.236184385391695</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>6270.8873288533696</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>16.5000896492751</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>13.751443859514501</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
excel actualizados a GKD only
</commit_message>
<xml_diff>
--- a/Docs importantes/Experimento 1/criterio1VScriterio3.xlsx
+++ b/Docs importantes/Experimento 1/criterio1VScriterio3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Investigacion-maxima-diversidad\Docs importantes\Experimento 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F95C25-4C4E-4F2B-BF4B-FF9100BB13D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4876EE-3571-4C0E-A6C8-89821FFA9959}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2850" windowWidth="24240" windowHeight="13140" xr2:uid="{D6DAAA7A-F829-4C97-A67F-BF00D45AC1A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6DAAA7A-F829-4C97-A67F-BF00D45AC1A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>GRASPConstructive_Criterion3_Seed_13_SolCount_100_alpha_0.75</t>
   </si>
@@ -142,21 +142,6 @@
   </si>
   <si>
     <t>GKD-c_1_n500_m50.txt</t>
-  </si>
-  <si>
-    <t>MDG-a_9_n500_m50.txt</t>
-  </si>
-  <si>
-    <t>MDG-b_12_n500_m50.txt</t>
-  </si>
-  <si>
-    <t>SOM-a_18_n50_m15.txt</t>
-  </si>
-  <si>
-    <t>SOM-a_33_n125_m12.txt</t>
-  </si>
-  <si>
-    <t>SOM-b_2_n100_m20.txt</t>
   </si>
   <si>
     <t>CV REF</t>
@@ -598,7 +583,7 @@
   <dimension ref="A2:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,28 +608,28 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -653,31 +638,31 @@
       </c>
       <c r="B3" s="3">
         <f>AVERAGE(B7:B30)</f>
-        <v>0.85717499431598154</v>
+        <v>0.82417036319055759</v>
       </c>
       <c r="C3" s="3">
         <f t="shared" ref="C3:H3" si="0">AVERAGE(C7:C30)</f>
-        <v>2.6302947230595938E-2</v>
+        <v>3.3224775063719153E-2</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" si="0"/>
-        <v>1.3445532721463394</v>
+        <v>1.3831656187615105</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" si="0"/>
-        <v>8530.6188581680381</v>
+        <v>4568.8103944684481</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>18.833333333333332</v>
+        <v>20.05263157894737</v>
       </c>
       <c r="G3" s="3">
         <f t="shared" si="0"/>
-        <v>0.97885344723100565</v>
+        <v>0.97724282400525331</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" si="0"/>
-        <v>650.08549043728738</v>
+        <v>399.17196085273042</v>
       </c>
       <c r="I3" s="4">
         <v>158.87799999999999</v>
@@ -689,31 +674,31 @@
       </c>
       <c r="B4" s="5">
         <f>AVERAGE(I7:I30)</f>
-        <v>2.8104135919600769E-2</v>
+        <v>3.5499961161600972E-2</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" ref="C4:H4" si="1">AVERAGE(J7:J30)</f>
-        <v>0.25950100626463851</v>
+        <v>0.29444204888036535</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="1"/>
-        <v>6.409964241117054E-2</v>
+        <v>7.7638121888715328E-2</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="1"/>
-        <v>13521.57842543016</v>
+        <v>8164.7301969509053</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="1"/>
-        <v>13.625</v>
+        <v>14.368421052631579</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="1"/>
-        <v>0.97912149871423715</v>
+        <v>0.97677510670222278</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="1"/>
-        <v>477.18548303161015</v>
+        <v>266.50292936363314</v>
       </c>
       <c r="I4" s="6">
         <v>161.56299999999999</v>
@@ -1660,239 +1645,84 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1347.0730136970301</v>
-      </c>
-      <c r="F26" s="1">
-        <v>20</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0.99373474835537701</v>
-      </c>
-      <c r="H26" s="1">
-        <v>65.877952533154797</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1">
-        <v>5.314684194851E-2</v>
-      </c>
-      <c r="K26" s="1">
-        <v>5.1749722726885002E-2</v>
-      </c>
-      <c r="L26" s="1">
-        <v>2110.8227359070002</v>
-      </c>
-      <c r="M26" s="1">
-        <v>11</v>
-      </c>
-      <c r="N26" s="1">
-        <v>0.99381568081191396</v>
-      </c>
-      <c r="O26" s="1">
-        <v>64.236184385391695</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0.96296296296296202</v>
-      </c>
-      <c r="C27" s="1">
-        <v>7.3236386176865804E-9</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0.99847243438411304</v>
-      </c>
-      <c r="E27" s="1">
-        <v>115942.077937724</v>
-      </c>
-      <c r="F27" s="1">
-        <v>27</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0.99349604420514603</v>
-      </c>
-      <c r="H27" s="1">
-        <v>7881.7900917910201</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1">
-        <v>4.5876098436471197E-2</v>
-      </c>
-      <c r="K27" s="1">
-        <v>1.1517379255616999E-2</v>
-      </c>
-      <c r="L27" s="1">
-        <v>166537.045853458</v>
-      </c>
-      <c r="M27" s="1">
-        <v>17</v>
-      </c>
-      <c r="N27" s="1">
-        <v>0.99588472701318997</v>
-      </c>
-      <c r="O27" s="1">
-        <v>6270.8873288533696</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E28" s="1">
-        <v>151.71047425936001</v>
-      </c>
-      <c r="F28" s="1">
-        <v>10</v>
-      </c>
-      <c r="G28" s="1">
-        <v>0.98104843495605598</v>
-      </c>
-      <c r="H28" s="1">
-        <v>21.497416085271201</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1">
-        <v>0.24841849148418399</v>
-      </c>
-      <c r="K28" s="1">
-        <v>0</v>
-      </c>
-      <c r="L28" s="1">
-        <v>152.40409563836101</v>
-      </c>
-      <c r="M28" s="1">
-        <v>14</v>
-      </c>
-      <c r="N28" s="1">
-        <v>0.98490381079916201</v>
-      </c>
-      <c r="O28" s="1">
-        <v>16.5000896492751</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1.5714285714285701</v>
-      </c>
-      <c r="E29" s="1">
-        <v>96.964356439637498</v>
-      </c>
-      <c r="F29" s="1">
-        <v>9</v>
-      </c>
-      <c r="G29" s="1">
-        <v>0.97098515699945798</v>
-      </c>
-      <c r="H29" s="1">
-        <v>18.100413972918801</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1">
-        <v>0.24971655328798101</v>
-      </c>
-      <c r="K29" s="1">
-        <v>0</v>
-      </c>
-      <c r="L29" s="1">
-        <v>164.48899546665601</v>
-      </c>
-      <c r="M29" s="1">
-        <v>6</v>
-      </c>
-      <c r="N29" s="1">
-        <v>0.99518083489864095</v>
-      </c>
-      <c r="O29" s="1">
-        <v>13.751443859514501</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1.2692307692307601</v>
-      </c>
-      <c r="E30" s="1">
-        <v>389.62931901238699</v>
-      </c>
-      <c r="F30" s="1">
-        <v>5</v>
-      </c>
-      <c r="G30" s="1">
-        <v>0.98560469292829</v>
-      </c>
-      <c r="H30" s="1">
-        <v>30.518639910653299</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1">
-        <v>3.6467236467236402E-2</v>
-      </c>
-      <c r="K30" s="1">
-        <v>0</v>
-      </c>
-      <c r="L30" s="1">
-        <v>423.24678778661098</v>
-      </c>
-      <c r="M30" s="1">
-        <v>6</v>
-      </c>
-      <c r="N30" s="1">
-        <v>0.970403888276552</v>
-      </c>
-      <c r="O30" s="1">
-        <v>23.520888102062401</v>
-      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>